<commit_message>
updates the cheat sheet
</commit_message>
<xml_diff>
--- a/cheat_sheet.xlsx
+++ b/cheat_sheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED1618C-917E-4E3B-9165-196B3CC400A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A380B30C-3F87-4DBE-AAA0-2B660F361048}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3525,7 +3525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09908FBF-4005-4292-9873-8B97BCEA93D6}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -3777,7 +3777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -4716,8 +4716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5564,114 +5564,114 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A61" s="29" t="s">
+      <c r="A61" s="66" t="s">
         <v>311</v>
       </c>
-      <c r="B61" s="30" t="s">
+      <c r="B61" s="70" t="s">
         <v>313</v>
       </c>
-      <c r="C61" s="31" t="s">
+      <c r="C61" s="71" t="s">
         <v>312</v>
       </c>
-      <c r="D61" s="32" t="s">
+      <c r="D61" s="69" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="29" t="s">
+      <c r="A62" s="66" t="s">
         <v>315</v>
       </c>
-      <c r="B62" s="30" t="s">
+      <c r="B62" s="70" t="s">
         <v>317</v>
       </c>
-      <c r="C62" s="31" t="s">
+      <c r="C62" s="71" t="s">
         <v>316</v>
       </c>
-      <c r="D62" s="32" t="s">
+      <c r="D62" s="69" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="29" t="s">
+      <c r="A63" s="66" t="s">
         <v>318</v>
       </c>
-      <c r="B63" s="30" t="s">
+      <c r="B63" s="70" t="s">
         <v>319</v>
       </c>
-      <c r="C63" s="31" t="s">
+      <c r="C63" s="71" t="s">
         <v>320</v>
       </c>
-      <c r="D63" s="32" t="s">
+      <c r="D63" s="69" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="29" t="s">
+      <c r="A64" s="66" t="s">
         <v>321</v>
       </c>
-      <c r="B64" s="30" t="s">
+      <c r="B64" s="70" t="s">
         <v>323</v>
       </c>
-      <c r="C64" s="31" t="s">
+      <c r="C64" s="71" t="s">
         <v>322</v>
       </c>
-      <c r="D64" s="32" t="s">
+      <c r="D64" s="69" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A65" s="29" t="s">
+      <c r="A65" s="66" t="s">
         <v>324</v>
       </c>
-      <c r="B65" s="30" t="s">
+      <c r="B65" s="70" t="s">
         <v>326</v>
       </c>
-      <c r="C65" s="31" t="s">
+      <c r="C65" s="71" t="s">
         <v>325</v>
       </c>
-      <c r="D65" s="32" t="s">
+      <c r="D65" s="69" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="29" t="s">
+      <c r="A66" s="66" t="s">
         <v>327</v>
       </c>
-      <c r="B66" s="30" t="s">
+      <c r="B66" s="70" t="s">
         <v>328</v>
       </c>
-      <c r="C66" s="31" t="s">
+      <c r="C66" s="71" t="s">
         <v>329</v>
       </c>
-      <c r="D66" s="32" t="s">
+      <c r="D66" s="69" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A67" s="29" t="s">
+      <c r="A67" s="66" t="s">
         <v>330</v>
       </c>
-      <c r="B67" s="30" t="s">
+      <c r="B67" s="70" t="s">
         <v>332</v>
       </c>
-      <c r="C67" s="31" t="s">
+      <c r="C67" s="71" t="s">
         <v>331</v>
       </c>
-      <c r="D67" s="32" t="s">
+      <c r="D67" s="69" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="29" t="s">
+      <c r="A68" s="66" t="s">
         <v>333</v>
       </c>
-      <c r="B68" s="30" t="s">
+      <c r="B68" s="70" t="s">
         <v>334</v>
       </c>
-      <c r="C68" s="31" t="s">
+      <c r="C68" s="71" t="s">
         <v>335</v>
       </c>
-      <c r="D68" s="32" t="s">
+      <c r="D68" s="69" t="s">
         <v>6</v>
       </c>
     </row>
@@ -6404,7 +6404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE05540-2EB2-490B-925E-8A2A980E466A}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A17" sqref="A17"/>
       <selection pane="topRight" activeCell="B17" sqref="B17"/>
@@ -6747,16 +6747,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B55396B-BB8C-4180-AD0D-7E5850126AB0}">
   <dimension ref="A2:L100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="17" customWidth="1"/>
     <col min="3" max="3" width="11" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="17" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" style="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.5703125" style="17" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="17" customWidth="1"/>
@@ -6777,7 +6777,7 @@
       <c r="D2" s="89"/>
       <c r="E2" s="89"/>
     </row>
-    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>578</v>
       </c>
@@ -6954,7 +6954,7 @@
       </c>
       <c r="I8" s="63">
         <f>COUNTIF(E4:E29, 2)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J8" s="63">
         <f>COUNTIF(E32:E58, 2)</f>
@@ -7038,7 +7038,7 @@
       </c>
       <c r="I10" s="63">
         <f>SUM(F4:F29)/6</f>
-        <v>11.947222222222225</v>
+        <v>11.322222222222225</v>
       </c>
       <c r="J10" s="63">
         <f>SUM(F32:F58)/6</f>
@@ -7068,11 +7068,11 @@
         <v>3.75</v>
       </c>
       <c r="E11" s="45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="43">
         <f t="shared" si="1"/>
-        <v>3.75</v>
+        <v>0</v>
       </c>
       <c r="G11" s="43"/>
       <c r="H11" s="59" t="s">
@@ -7080,11 +7080,11 @@
       </c>
       <c r="I11" s="64">
         <f ca="1">TODAY() +I10</f>
-        <v>43807.947222222225</v>
+        <v>43808.322222222225</v>
       </c>
       <c r="J11" s="64">
         <f ca="1">I11+J10</f>
-        <v>43824.025000000001</v>
+        <v>43824.4</v>
       </c>
       <c r="K11" s="64"/>
       <c r="L11" s="64"/>
@@ -7116,7 +7116,7 @@
       </c>
       <c r="I12" s="65">
         <f>I8/I7</f>
-        <v>0.30769230769230771</v>
+        <v>0.34615384615384615</v>
       </c>
       <c r="J12" s="65">
         <f>J8/J7</f>
@@ -7158,7 +7158,7 @@
       </c>
       <c r="I13" s="86">
         <f>AVERAGE(I12:L12)</f>
-        <v>0.10701566951566951</v>
+        <v>0.11663105413105412</v>
       </c>
       <c r="J13" s="87"/>
       <c r="K13" s="87"/>

</xml_diff>

<commit_message>
added changes to the repo
</commit_message>
<xml_diff>
--- a/cheat_sheet.xlsx
+++ b/cheat_sheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217435E1-55EA-48D7-B1A9-68151065962F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24824A6C-5D58-421C-BACA-0821497EEB49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27660" windowHeight="14670" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,16 @@
     <sheet name="Samplers" sheetId="5" r:id="rId7"/>
     <sheet name="LDP" sheetId="8" r:id="rId8"/>
     <sheet name="CSS Selectors" sheetId="9" r:id="rId9"/>
+    <sheet name="CSS Transitions" sheetId="10" r:id="rId10"/>
+    <sheet name="SASS" sheetId="11" r:id="rId11"/>
+    <sheet name="Questions" sheetId="12" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'CSS Selectors'!$A$2:$D$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">HTML!$A$2:$D$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="932">
   <si>
     <t>HTML</t>
   </si>
@@ -2638,6 +2642,560 @@
   </si>
   <si>
     <t>&lt;select id="job" name="user_job"&gt;&lt;/select&gt;</t>
+  </si>
+  <si>
+    <t>Transition Duration</t>
+  </si>
+  <si>
+    <t>The transition-duration CSS property sets the length of time a transition animation should take to complete. By default, the value is 0s, meaning that no animation will occur.</t>
+  </si>
+  <si>
+    <t>The transition-property CSS property sets the CSS properties to which a transition effect should be applied.</t>
+  </si>
+  <si>
+    <t>button:active {
+transition-property: margin-right, color;
+}</t>
+  </si>
+  <si>
+    <t>Transition Property</t>
+  </si>
+  <si>
+    <t>List of animatable properties</t>
+  </si>
+  <si>
+    <t>Certain CSS properties can be animated using CSS Animations or CSS Transitions. Animation means that their values can be made to change gradually over a given amount of time.</t>
+  </si>
+  <si>
+    <t>button:hover {
+  background: #d36a62;
+  transition-duration: 2s, 0.4s;
+}</t>
+  </si>
+  <si>
+    <t>Transition Delay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The transition-delay CSS property specifies the duration to wait before starting a property's transition effect when its value changes.
+</t>
+  </si>
+  <si>
+    <t>button {
+  transition-duration: 2s, 1s;
+  transition-property: background, color;
+  transition-delay: 0s, 2s;
+}</t>
+  </si>
+  <si>
+    <t>button {
+  transition-duration: 2s, 1s;
+  transition-property: background, color;
+  transition-delay: 0s, 2s;
+  transition-timing-function: ease-in, ease-in-out;
+}</t>
+  </si>
+  <si>
+    <t>The transition-timing-function CSS property sets how intermediate values are calculated for CSS properties being affected by a transition effect.</t>
+  </si>
+  <si>
+    <t>Transition Timing Function</t>
+  </si>
+  <si>
+    <t>Transition (SHORTHAND)</t>
+  </si>
+  <si>
+    <t>button {
+  transition: background 2s ease-in 0s,
+                     color 1s ease-in-out 2s;
+}</t>
+  </si>
+  <si>
+    <t>Transform</t>
+  </si>
+  <si>
+    <t>The &lt;transform-function&gt; CSS data type represents a transformation that affects an element's appearance. Transformation functions can rotate, resize, distort, or move an element in 2D or 3D space. It is used in the transform property.</t>
+  </si>
+  <si>
+    <t>button:hover {
+  transform: rotate(360deg);
+}</t>
+  </si>
+  <si>
+    <t>Transform - rotate</t>
+  </si>
+  <si>
+    <t>button:hover {
+  transform: &lt;value&gt;;
+}</t>
+  </si>
+  <si>
+    <t>The rotate() CSS function defines a transformation that rotates an element around a fixed point on the 2D plane, without deforming it. Its result is a &lt;transform-function&gt; data type.</t>
+  </si>
+  <si>
+    <t>Transform - skew (SHORTHAND)</t>
+  </si>
+  <si>
+    <t>button:hover {
+  transform: skew(10deg, 10deg);
+}</t>
+  </si>
+  <si>
+    <t>The skew() CSS function defines a transformation that skews an element on the 2D plane. Its result is a &lt;transform-function&gt; data type.
+&lt;transform&gt;: &lt;skew&gt;(&lt;x-axis value&gt; &lt;y-axis value&gt;);</t>
+  </si>
+  <si>
+    <t>The transition CSS property is a shorthand property for transition-property, transition-duration, transition-timing-function, and transition-delay.
+&lt;transition&gt;: &lt;transition-property-value&gt; &lt;transition-duration-value&gt; &lt;transition-timing-function-value&gt; &lt;transition-delay-value&gt;;</t>
+  </si>
+  <si>
+    <t>Transform - scale (SHORTHAND)</t>
+  </si>
+  <si>
+    <t>button:hover {
+  transform: scale(1.5 1.5);
+}</t>
+  </si>
+  <si>
+    <t>The scale() CSS function defines a transformation that resizes an element on the 2D plane. Because the amount of scaling is defined by a vector, it can resize the horizontal and vertical dimensions at different scales. Its result is a &lt;transform-function&gt; data type.
+&lt;transform&gt;: &lt;scale&gt;(&lt;x-axis value&gt; &lt;y-axis value&gt;);</t>
+  </si>
+  <si>
+    <t>button:hover {
+  transform: scale(1.5 1.5);
+  transform-origin: left 50%;
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The transform-origin CSS property sets the origin for an element's transformations.
+&lt;transform-origin&gt;: &lt;x-axis value&gt;  &lt;y-axis value&gt;;
+</t>
+  </si>
+  <si>
+    <t>Transform Origin</t>
+  </si>
+  <si>
+    <t>Transform - translate (SHORTHAND)</t>
+  </si>
+  <si>
+    <t>button:hover {
+  transform: translate(150px 20px);
+}</t>
+  </si>
+  <si>
+    <t>The translate() CSS function repositions an element in the horizontal and/or vertical directions. Its result is a &lt;transform-function&gt; data type.
+&lt;transform&gt;: &lt;translate&gt;(&lt;x-axis value&gt;  &lt;y-axis value&gt;);</t>
+  </si>
+  <si>
+    <t>Modifying Cubic Bezier</t>
+  </si>
+  <si>
+    <t>Perspective</t>
+  </si>
+  <si>
+    <t>.content {
+  persepective: 700px;
+}</t>
+  </si>
+  <si>
+    <t>The perspective CSS property determines the distance between the z=0 plane and the user in order to give a 3D-positioned element some perspective. Each 3D element with z&gt;0 becomes larger; each 3D-element with z&lt;0 becomes smaller. The strength of the effect is determined by the value of this property.</t>
+  </si>
+  <si>
+    <t>Transform Style</t>
+  </si>
+  <si>
+    <t>.button_container {
+  transition: transform 5s ease-out;
+  transform-style: preserve-3d;
+}</t>
+  </si>
+  <si>
+    <t>Backface Visibility</t>
+  </si>
+  <si>
+    <t>.button_1 {
+  z-index: 0;
+  backface-visibility: hidden;
+}</t>
+  </si>
+  <si>
+    <t>The backface-visibility CSS property sets whether the back face of an element is visible when turned towards the user.</t>
+  </si>
+  <si>
+    <t>The transform-style CSS property sets whether children of an element are positioned in the 3D space or are flattened in the plane of the element.</t>
+  </si>
+  <si>
+    <t>Rotate 3D</t>
+  </si>
+  <si>
+    <t>.button_container:hover {
+  transform: rotate3d(1, 0, 1, 180deg);
+}</t>
+  </si>
+  <si>
+    <t>The rotate3d() CSS function defines a transformation that rotates an element around a fixed axis in 3D space, without deforming it. Its result is a &lt;transform-function&gt; data type.
+&lt;transform&gt;:  &lt;rotate3d&gt;(&lt;x-axis&gt;,  &lt;y-axis&gt;,  &lt;z-axis&gt;,  &lt;angle&gt;);</t>
+  </si>
+  <si>
+    <t>Perspective Origin</t>
+  </si>
+  <si>
+    <t>.content {
+  persepective: 700px;
+  perspective-origin: bottom right;
+}</t>
+  </si>
+  <si>
+    <t>The perspective-origin CSS property determines the position at which the viewer is looking. It is used as the vanishing point by the perspective property.
+&lt;perspective-origin&gt;:  &lt;x-axis&gt; &lt;y-axis&gt;;</t>
+  </si>
+  <si>
+    <t>Transform - translate 3d (SHORTHAND)</t>
+  </si>
+  <si>
+    <t>button:hover {
+  transform: translate3d(42px, -62px, -135px);
+}</t>
+  </si>
+  <si>
+    <t>The translate3d() CSS function repositions an element in 3D space. Its result is a &lt;transform-function&gt; data type.</t>
+  </si>
+  <si>
+    <t>Linking a SASS file to an output</t>
+  </si>
+  <si>
+    <t>sass &lt;sass file name&gt;.scss  &lt;output file name and path&gt;.css</t>
+  </si>
+  <si>
+    <t>SASS Variables</t>
+  </si>
+  <si>
+    <t>Sass variables are simple: you assign a value to a name that begins with $, and then you can refer to that name instead of the value itself. But despite their simplicity, they're one of the most useful tools Sass brings to the table. Variables make it possible to reduce repetition, do complex math, configure libraries, and much more</t>
+  </si>
+  <si>
+    <t>$placeholder_color: rgba(145, 149, 148, 0.9);
+$main_background_color: rgba(251, 216, 183, 0.2);</t>
+  </si>
+  <si>
+    <t>SASS Nesting</t>
+  </si>
+  <si>
+    <t>Rather than repeating the same selectors over and over again, you can write one style rules inside another. Sass will automatically combine the outer rule’s selector with the inner rule’s.</t>
+  </si>
+  <si>
+    <t>Parent Selector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When a parent selector is used in an inner selector, it’s replaced with the corresponding outer selector. This happens instead of the normal nesting behavior.
+</t>
+  </si>
+  <si>
+    <t>Mixins allow you to define styles that can be re-used throughout your stylesheet. They make it easy to avoid using non-semantic classes like .float-left, and to distribute collections of styles in libraries.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+@mixin placeholder_styles {
+  font: 1.3rem;
+  &amp;::placeholder {
+    color: $placeholder_color;
+    font-style: italic;
+    @content;
+  }
+}
+input {
+  @include placeholder_styles {
+    text-align: right;
+  }
+}</t>
+  </si>
+  <si>
+    <t>In addition to taking arguments, a mixin can take an entire block of styles, known as a content block. A mixin can declare that it takes a content block by including the @content at-rule in its body. The content block is passed in using curly braces like any other block in Sass, and it’s injected in place of the @content rule.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  @mixin and @include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  @extend</t>
+  </si>
+  <si>
+    <t>Unlike mixins, which copy styles into the current style rule, @extend updates style rules that contain the extended selector so that they contain the extending selector as well. When extending selectors, Sass does intelligent unification:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mixins - @content </t>
+  </si>
+  <si>
+    <t>%placeholder_selectors</t>
+  </si>
+  <si>
+    <t>Unlike class selectors, placeholders don’t clutter up the CSS if they aren’t extended and they don’t mandate that users of a library use specific class names for their HTML.</t>
+  </si>
+  <si>
+    <t>%placeholder {
+  &amp;::placeholder {
+    color: rgba(145, 149, 148, 0.9);
+    font-style: italic;
+  }
+}</t>
+  </si>
+  <si>
+    <t>input {
+  @extend %placeholder;
+  text-align: right;
+}</t>
+  </si>
+  <si>
+    <t>.input_container {
+  &gt; input,
+  &gt; select,
+  &gt; textarea {
+    width: 100%;
+    padding: 15px;
+  }
+}</t>
+  </si>
+  <si>
+    <t>.input_container {
+  margin: 5px 0;
+  border-radius: 5px;
+  &amp;:nth-of-type(-1n-6) {
+    width: 100%;
+  }
+  &amp;:nth-of-type(7) {
+    width: 50%;
+  }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+@mixin flex_styles {
+  display: flex;
+  flex-direction: row;
+}
+.flex1,
+.flex2 {
+  @include flex_styles;
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  @import partials</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @import  "partials/_variables.scss",
+                      "partials/_placeholders.scss",
+                      "partials/_styles.scss";</t>
+  </si>
+  <si>
+    <t>When Sass imports a file, that file is evaluated as though its contents appeared directly in place of the @import. Any mixins, functions, and variables from the imported file are made available, and all its CSS is included at the exact point where the @import was written. What’s more, any mixins, functions, or variables that were defined before the @import (including from other @imports) are available in the imported stylesheet.</t>
+  </si>
+  <si>
+    <t>Nesting media queries</t>
+  </si>
+  <si>
+    <t>If a CSS at-rule is nested within a style rule, the two automatically swap positions so that the at-rule is at the top level of the CSS output and the style rule is within it. This makes it easy to add conditional styling without having to rewrite the style rule’s selector.</t>
+  </si>
+  <si>
+    <t>.banner,
+.newsletter_signup {
+  width: 90%;
+  max-width: 500px;
+  margin: 0 auto;
+  @media only screen and (min-width: $break_m) {
+    width: 750px;
+    max-width: 800px;
+    margin: 0 auto 3px;
+  }
+}</t>
+  </si>
+  <si>
+    <t>Color Functions</t>
+  </si>
+  <si>
+    <t>$base: 3acec2;
+$base-dark: darken($base, 50%)
+$base-light: lighten($base, 100%)
+$base-complement: complement($base)
+$base-complement-dark: darken($base-complement, 10%)</t>
+  </si>
+  <si>
+    <t>Custom functions @function</t>
+  </si>
+  <si>
+    <t>Functions are defined using the @function at-rule, which is written @function &lt;name&gt;(&lt;arguments...&gt;) { ... }. A function’s name can be any Sass identifier. It can only contain universal statements, as well as the @return at-rule which indicates the value to use as the result of the function call. Functions are called using the normal CSS function syntax.</t>
+  </si>
+  <si>
+    <t>$container_width: 1000px;
+$gutter: 10px;
+@function flex_item_width ($number: 2) {
+  $gutter_pc: ($gutter * 2) * $number;
+  $remaining_space: $container_width - $gutter_pc;
+  @return ($remaining_space / $container_width * 100% ) / $number;
+}
+flex_item {
+  width: flex_item_width(3)
+}</t>
+  </si>
+  <si>
+    <t>Mixin arguments @mixin()</t>
+  </si>
+  <si>
+    <t>Mixins can also take arguments, which allows their behavior to be customized each time they’re called. The arguments are specified in the @mixin rule after the mixin’s name, as a list of variable names surrounded by parentheses. The mixin must then be included with the same number of arguments in the form of SassScript expressions. The values of these expression are available within the mixin’s body as the corresponding variables.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+@mixin flex_styles(
+  $display: flex,
+  $flex_direction: null,
+  $align_items: null,
+  $flex_wrap: null
+) {
+  display: $display;
+  flex-direction: $flex_direction;
+  align-items: $align_items;
+  flex-wrap: $flex_wrap;
+}
+.flex1,
+.flex2 {
+  @include flex_styles($flex_direction: row,
+                       $flex_wrap: wrap,
+                       $align_items: center);
+}</t>
+  </si>
+  <si>
+    <t>Numeric Operators</t>
+  </si>
+  <si>
+    <t>$break_m: 768px;
+$break_l: 1024px;
+@mixin break($screen_width) {
+  @if $screen_width == "m" {
+    @media only screen and (min-width: $break_m) {
+      @content;
+    }
+  }
+  @else if $screen_width == "l" {
+    @media only screen and (min-width: $break_l) {
+      @content;
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  @if and @else</t>
+  </si>
+  <si>
+    <t>The @if rule is written @if &lt;expression&gt; { ... }, and it controls whether or not its block gets evaluated (including emitting any styles as CSS). The expression usually returns either true or false—if the expression returns true, the block is evaluated, and if the expression returns false it’s not.</t>
+  </si>
+  <si>
+    <t>Maps and its functions $map: ( "m": 768px);</t>
+  </si>
+  <si>
+    <t>$break: (
+ "m": 768px,
+ "l": 1024px,
+);
+@mixin break($screen_width) {
+  $value: map-get($break, $screen_width);
+  @if $screen_width == "m" {
+    @media only screen and (min-width: $value) {
+      @content;
+    }
+  }
+  @else if $screen_width == "l" {
+    @media only screen and (min-width: $value) {
+      @content;
+    }
+  }
+}</t>
+  </si>
+  <si>
+    <t>Maps in Sass hold pairs of keys and values, and make it easy to look up a value by its corresponding key. They’re written (&lt;expression&gt;: &lt;expression&gt;, &lt;expression&gt;: &lt;expression&gt;). The expression before the : is the key, and the expression after is the value associated with that key. The keys must be unique, but the values may be duplicated. Unlike lists, maps must be written with parentheses around them. A map with no pairs is written ().</t>
+  </si>
+  <si>
+    <t>For loops @for</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @for $index from 1 through 2 {
+  .box#{$index} {
+    background: adjust-hue(tomato, $index * 100);
+  }
+}</t>
+  </si>
+  <si>
+    <t>The @for rule, written @for &lt;variable&gt; from &lt;expression&gt; to &lt;expression&gt; { ... } or @for &lt;variable&gt; from &lt;expression&gt; through &lt;expression&gt; { ... }, counts up or down from one number (the result of the first expression) to another (the result of the second) and evaluates a block for each number in between. Each number along the way is assigned to the given variable name. If to is used, the final number is excluded; if through is used, it's included.</t>
+  </si>
+  <si>
+    <t>Interpolation</t>
+  </si>
+  <si>
+    <t>Interpolation can be used almost anywhere in a Sass stylesheet to embed the result of a SassScript expression into a chunk of CSS. Just wrap an expression in #{} in any of the following places:</t>
+  </si>
+  <si>
+    <t>SASS Lists</t>
+  </si>
+  <si>
+    <t>$sizes: (40px, 50px, 80px);
+ @each $size in $sizes {
+  .icon-#{$size} {
+    font-size: $size;
+    height: $size;
+    width: $size;
+  }
+}</t>
+  </si>
+  <si>
+    <t>Lists contain a sequence of other values. In Sass, elements in lists can be separated by commas (Helvetica, Arial, sans-serif) or by spaces (10px 15px 0 0), as long as it’s consistent within the list.</t>
+  </si>
+  <si>
+    <t>$teachers: (
+  "mathew",
+  "alena",
+  "joel",
+  "daniel",
+  "nick",
+);
+@each $teacher in $teachers {
+  .image-#{$teacher} {
+    background: url("images/#{$teacher}.jpg");
+  }
+}</t>
+  </si>
+  <si>
+    <t>Each Loops @each</t>
+  </si>
+  <si>
+    <t>The @each rule makes it easy to emit styles or evaluate code for each element of a list or each pair in a map. It’s great for repetitive styles that only have a few variations between them. It’s usually written @each &lt;variable&gt; in &lt;expression&gt; { ... }, where the expression returns a list. The block is evaluated for each element of the list in turn, which is assigned to the given variable name.</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>HTML / CSS</t>
+  </si>
+  <si>
+    <t>Form Styling / Focus State styling</t>
+  </si>
+  <si>
+    <t>to apply a certain transition style which would basically fade out other elements on the page when a particular form element is in focus by increasing the opacity of focused element and decreasing the opacity of the other page elements.  When thinking about it theoretically I assumed that this could be achieved by targeting parent elements however when looking it up online I found out that CSS does not have this functionality. Hence is this possible and how would one do it ?</t>
+  </si>
+  <si>
+    <t>Achieveable through Javascript</t>
+  </si>
+  <si>
+    <t>SASS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looping through a theme list </t>
+  </si>
+  <si>
+    <t>Is it possible to create a loop to cycle through a map however stop at a certain index in the map ? For example I have a color theme map with five colors (1-12) and I would like to create a mixin to accept a number argument which would be the stopping point. Then the mixin would execute the loop however stop the map loop when it reaches the mixin argument number.</t>
   </si>
 </sst>
 </file>
@@ -3645,7 +4203,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4002,6 +4560,761 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58C87AB-222A-4E13-8A46-2201C051A1C5}">
+  <dimension ref="A2:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.85546875" customWidth="1"/>
+    <col min="2" max="2" width="58" customWidth="1"/>
+    <col min="3" max="3" width="110.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="s">
+        <v>812</v>
+      </c>
+      <c r="B3" s="80" t="s">
+        <v>819</v>
+      </c>
+      <c r="C3" s="79" t="s">
+        <v>813</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
+        <v>816</v>
+      </c>
+      <c r="B4" s="80" t="s">
+        <v>815</v>
+      </c>
+      <c r="C4" s="79" t="s">
+        <v>814</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="56" t="s">
+        <v>817</v>
+      </c>
+      <c r="B5" s="80"/>
+      <c r="C5" s="79" t="s">
+        <v>818</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="56" t="s">
+        <v>820</v>
+      </c>
+      <c r="B6" s="80" t="s">
+        <v>822</v>
+      </c>
+      <c r="C6" s="79" t="s">
+        <v>821</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="56" t="s">
+        <v>825</v>
+      </c>
+      <c r="B7" s="80" t="s">
+        <v>823</v>
+      </c>
+      <c r="C7" s="79" t="s">
+        <v>824</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A8" s="56" t="s">
+        <v>826</v>
+      </c>
+      <c r="B8" s="80" t="s">
+        <v>827</v>
+      </c>
+      <c r="C8" s="79" t="s">
+        <v>837</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="56" t="s">
+        <v>828</v>
+      </c>
+      <c r="B9" s="80" t="s">
+        <v>832</v>
+      </c>
+      <c r="C9" s="79" t="s">
+        <v>829</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="56" t="s">
+        <v>831</v>
+      </c>
+      <c r="B10" s="80" t="s">
+        <v>830</v>
+      </c>
+      <c r="C10" s="79" t="s">
+        <v>833</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="56" t="s">
+        <v>834</v>
+      </c>
+      <c r="B11" s="80" t="s">
+        <v>835</v>
+      </c>
+      <c r="C11" s="79" t="s">
+        <v>836</v>
+      </c>
+      <c r="D11" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A12" s="56" t="s">
+        <v>838</v>
+      </c>
+      <c r="B12" s="80" t="s">
+        <v>839</v>
+      </c>
+      <c r="C12" s="79" t="s">
+        <v>840</v>
+      </c>
+      <c r="D12" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A13" s="56" t="s">
+        <v>843</v>
+      </c>
+      <c r="B13" s="80" t="s">
+        <v>841</v>
+      </c>
+      <c r="C13" s="79" t="s">
+        <v>842</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="56" t="s">
+        <v>844</v>
+      </c>
+      <c r="B14" s="80" t="s">
+        <v>845</v>
+      </c>
+      <c r="C14" s="79" t="s">
+        <v>846</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="56" t="s">
+        <v>863</v>
+      </c>
+      <c r="B15" s="80" t="s">
+        <v>864</v>
+      </c>
+      <c r="C15" s="79" t="s">
+        <v>865</v>
+      </c>
+      <c r="D15" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="56" t="s">
+        <v>847</v>
+      </c>
+      <c r="B16" s="80"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="56" t="s">
+        <v>848</v>
+      </c>
+      <c r="B17" s="80" t="s">
+        <v>849</v>
+      </c>
+      <c r="C17" s="79" t="s">
+        <v>850</v>
+      </c>
+      <c r="D17" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A18" s="56" t="s">
+        <v>851</v>
+      </c>
+      <c r="B18" s="80" t="s">
+        <v>852</v>
+      </c>
+      <c r="C18" s="79" t="s">
+        <v>856</v>
+      </c>
+      <c r="D18" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
+        <v>853</v>
+      </c>
+      <c r="B19" s="80" t="s">
+        <v>854</v>
+      </c>
+      <c r="C19" s="79" t="s">
+        <v>855</v>
+      </c>
+      <c r="D19" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="56" t="s">
+        <v>857</v>
+      </c>
+      <c r="B20" s="80" t="s">
+        <v>858</v>
+      </c>
+      <c r="C20" s="79" t="s">
+        <v>859</v>
+      </c>
+      <c r="D20" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A21" s="56" t="s">
+        <v>860</v>
+      </c>
+      <c r="B21" s="80" t="s">
+        <v>861</v>
+      </c>
+      <c r="C21" s="79" t="s">
+        <v>862</v>
+      </c>
+      <c r="D21" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{EB5A99D5-13EA-48F1-9217-B84777B42FCB}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{62499128-6C43-4568-ADD8-75ADBD896487}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{D671F6DD-3735-4FF1-8402-5BA21519626D}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{3AD9443F-F59A-4778-8654-BA3D0FC3CCA0}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{C5B05BE4-3FAD-4B67-85AD-FD1F8F8BB316}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{C15A633C-290B-49E2-B392-A41C1706A8E7}"/>
+    <hyperlink ref="D9" r:id="rId7" xr:uid="{645C2233-BE19-4B21-A2FE-76A3D36DA1FC}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{17E2A589-4ED1-4B3B-9BCF-A1866E71668A}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{D019EF1E-E569-4136-AE7B-29206B846190}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{A390E101-F83E-45CB-9DD1-41ADE4E563C7}"/>
+    <hyperlink ref="D13" r:id="rId11" xr:uid="{FDC48A72-9199-4A21-936D-821ED88A65CE}"/>
+    <hyperlink ref="D14" r:id="rId12" xr:uid="{C198E2C0-0EC5-49F0-9ACC-8DAB8A02783E}"/>
+    <hyperlink ref="D16" r:id="rId13" location=".17,.67,.83,.67" xr:uid="{C398C20F-83CD-4158-A01E-50B7C87756EA}"/>
+    <hyperlink ref="D17" r:id="rId14" xr:uid="{86EFF247-2FA8-4C59-8122-F8DFA68C4FEB}"/>
+    <hyperlink ref="D18" r:id="rId15" xr:uid="{90D81EBC-D2BD-40DA-BFB0-9C3A34990E30}"/>
+    <hyperlink ref="D19" r:id="rId16" xr:uid="{99EF6861-5694-42B1-8F49-366224A89A95}"/>
+    <hyperlink ref="D20" r:id="rId17" xr:uid="{E5C179D4-8AB1-460C-9E0B-440980945740}"/>
+    <hyperlink ref="D21" r:id="rId18" xr:uid="{5383C8E5-9A75-4036-ADB2-91B4FE778E8D}"/>
+    <hyperlink ref="D15" r:id="rId19" xr:uid="{01606FAD-0E97-41CF-B964-179F74425AEA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2567DD-FB9D-4130-8587-5DE1233956C1}">
+  <dimension ref="A2:D22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.85546875" customWidth="1"/>
+    <col min="2" max="2" width="58" customWidth="1"/>
+    <col min="3" max="3" width="110.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="s">
+        <v>866</v>
+      </c>
+      <c r="B3" s="80" t="s">
+        <v>867</v>
+      </c>
+      <c r="C3" s="79"/>
+      <c r="D3" s="59"/>
+    </row>
+    <row r="4" spans="1:4" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="56" t="s">
+        <v>868</v>
+      </c>
+      <c r="B4" s="80" t="s">
+        <v>870</v>
+      </c>
+      <c r="C4" s="79" t="s">
+        <v>869</v>
+      </c>
+      <c r="D4" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="126" x14ac:dyDescent="0.25">
+      <c r="A5" s="56" t="s">
+        <v>871</v>
+      </c>
+      <c r="B5" s="80" t="s">
+        <v>886</v>
+      </c>
+      <c r="C5" s="79" t="s">
+        <v>872</v>
+      </c>
+      <c r="D5" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="189" x14ac:dyDescent="0.25">
+      <c r="A6" s="56" t="s">
+        <v>873</v>
+      </c>
+      <c r="B6" s="80" t="s">
+        <v>887</v>
+      </c>
+      <c r="C6" s="79" t="s">
+        <v>874</v>
+      </c>
+      <c r="D6" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="56" t="s">
+        <v>878</v>
+      </c>
+      <c r="B7" s="80" t="s">
+        <v>888</v>
+      </c>
+      <c r="C7" s="79" t="s">
+        <v>875</v>
+      </c>
+      <c r="D7" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="236.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="56" t="s">
+        <v>881</v>
+      </c>
+      <c r="B8" s="80" t="s">
+        <v>876</v>
+      </c>
+      <c r="C8" s="79" t="s">
+        <v>877</v>
+      </c>
+      <c r="D8" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A9" s="56" t="s">
+        <v>879</v>
+      </c>
+      <c r="B9" s="80" t="s">
+        <v>885</v>
+      </c>
+      <c r="C9" s="79" t="s">
+        <v>880</v>
+      </c>
+      <c r="D9" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="56" t="s">
+        <v>882</v>
+      </c>
+      <c r="B10" s="80" t="s">
+        <v>884</v>
+      </c>
+      <c r="C10" s="79" t="s">
+        <v>883</v>
+      </c>
+      <c r="D10" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="63" x14ac:dyDescent="0.25">
+      <c r="A11" s="56" t="s">
+        <v>889</v>
+      </c>
+      <c r="B11" s="80" t="s">
+        <v>890</v>
+      </c>
+      <c r="C11" s="79" t="s">
+        <v>891</v>
+      </c>
+      <c r="D11" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="56" t="s">
+        <v>892</v>
+      </c>
+      <c r="B12" s="80" t="s">
+        <v>894</v>
+      </c>
+      <c r="C12" s="79" t="s">
+        <v>893</v>
+      </c>
+      <c r="D12" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="56" t="s">
+        <v>895</v>
+      </c>
+      <c r="B13" s="80" t="s">
+        <v>896</v>
+      </c>
+      <c r="C13" s="79"/>
+      <c r="D13" s="81"/>
+    </row>
+    <row r="14" spans="1:4" ht="204.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="56" t="s">
+        <v>897</v>
+      </c>
+      <c r="B14" s="80" t="s">
+        <v>899</v>
+      </c>
+      <c r="C14" s="79" t="s">
+        <v>898</v>
+      </c>
+      <c r="D14" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="299.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="56" t="s">
+        <v>900</v>
+      </c>
+      <c r="B15" s="80" t="s">
+        <v>902</v>
+      </c>
+      <c r="C15" s="79" t="s">
+        <v>901</v>
+      </c>
+      <c r="D15" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="56" t="s">
+        <v>903</v>
+      </c>
+      <c r="B16" s="80"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="236.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="56" t="s">
+        <v>905</v>
+      </c>
+      <c r="B17" s="80" t="s">
+        <v>904</v>
+      </c>
+      <c r="C17" s="79" t="s">
+        <v>906</v>
+      </c>
+      <c r="D17" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="299.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="56" t="s">
+        <v>907</v>
+      </c>
+      <c r="B18" s="80" t="s">
+        <v>908</v>
+      </c>
+      <c r="C18" s="79" t="s">
+        <v>909</v>
+      </c>
+      <c r="D18" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="56" t="s">
+        <v>910</v>
+      </c>
+      <c r="B19" s="80" t="s">
+        <v>911</v>
+      </c>
+      <c r="C19" s="79" t="s">
+        <v>912</v>
+      </c>
+      <c r="D19" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="56" t="s">
+        <v>913</v>
+      </c>
+      <c r="B20" s="80"/>
+      <c r="C20" s="79" t="s">
+        <v>914</v>
+      </c>
+      <c r="D20" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="56" t="s">
+        <v>915</v>
+      </c>
+      <c r="B21" s="80" t="s">
+        <v>916</v>
+      </c>
+      <c r="C21" s="79" t="s">
+        <v>917</v>
+      </c>
+      <c r="D21" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="204.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="56" t="s">
+        <v>919</v>
+      </c>
+      <c r="B22" s="80" t="s">
+        <v>918</v>
+      </c>
+      <c r="C22" s="79" t="s">
+        <v>920</v>
+      </c>
+      <c r="D22" s="81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{5FE5A86E-9D27-4070-A61D-0DC5FC79E656}"/>
+    <hyperlink ref="D5" r:id="rId2" location="nesting" xr:uid="{1C03DB99-5BA2-45FD-8E25-EAB33B6D28BD}"/>
+    <hyperlink ref="D6" r:id="rId3" xr:uid="{CEDBF147-AAED-44B7-B893-B35D5CD22D45}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{7E214994-18A3-4442-B612-BA26D5D27A48}"/>
+    <hyperlink ref="D8" r:id="rId5" location="content-blocks" xr:uid="{2C91E3B9-9525-4FB5-9864-3A96583AE862}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{53B78FB8-98AD-48EF-A449-E82000AAF4A6}"/>
+    <hyperlink ref="D10" r:id="rId7" xr:uid="{20B7F0B1-9055-4F82-A5C6-6CA8BEEDC13A}"/>
+    <hyperlink ref="D11" r:id="rId8" location="partials" xr:uid="{5C0AD2FC-70FC-458E-80DC-03E99A8CAA71}"/>
+    <hyperlink ref="D12" r:id="rId9" location="media" xr:uid="{6293809B-6861-4622-A48E-4C60CA96C9F0}"/>
+    <hyperlink ref="D14" r:id="rId10" xr:uid="{28293FC4-556C-4165-B7A6-4A683B518A8D}"/>
+    <hyperlink ref="D15" r:id="rId11" location="arguments" xr:uid="{283551E3-DD0D-48DD-960D-2F0202A8217F}"/>
+    <hyperlink ref="D16" r:id="rId12" xr:uid="{6B1BE6F5-C82E-4F2C-977C-BA2C842C8938}"/>
+    <hyperlink ref="D17" r:id="rId13" xr:uid="{6099CB43-837B-49A3-B63E-672C02B6B791}"/>
+    <hyperlink ref="D18" r:id="rId14" xr:uid="{8BE4AE5C-B138-4046-B447-86D439AB040C}"/>
+    <hyperlink ref="D19" r:id="rId15" xr:uid="{F717025E-195C-4FCE-8A74-3A6D038A8412}"/>
+    <hyperlink ref="D20" r:id="rId16" xr:uid="{6EDCD131-9E60-4873-9427-333DD9B3AEDB}"/>
+    <hyperlink ref="D21" r:id="rId17" xr:uid="{C81ECE98-5384-498D-98FE-4E2847319C92}"/>
+    <hyperlink ref="D22" r:id="rId18" xr:uid="{7E9E02ED-A58B-4962-BA1B-527B605A5556}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AB73040-3CFA-4428-B65C-7649A446D17C}">
+  <dimension ref="A2:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="3" max="3" width="125.42578125" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>921</v>
+      </c>
+      <c r="B2" t="s">
+        <v>922</v>
+      </c>
+      <c r="C2" t="s">
+        <v>923</v>
+      </c>
+      <c r="D2" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>925</v>
+      </c>
+      <c r="B3" t="s">
+        <v>926</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>927</v>
+      </c>
+      <c r="D3" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>929</v>
+      </c>
+      <c r="B4" t="s">
+        <v>930</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="16"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="16"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="16"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="16"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="16"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="16"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="16"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="16"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="16"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="16"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="16"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="16"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="16"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="16"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="16"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="16"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="16"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5352,8 +6665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D11"/>
+    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6569,7 +7882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -7384,7 +8697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B55396B-BB8C-4180-AD0D-7E5850126AB0}">
   <dimension ref="A2:L101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -7717,11 +9030,11 @@
       </c>
       <c r="I11" s="49">
         <f ca="1">TODAY() +I10</f>
-        <v>43812.261111111111</v>
+        <v>43818.261111111111</v>
       </c>
       <c r="J11" s="49">
         <f ca="1">I11+J10</f>
-        <v>43828.338888888888</v>
+        <v>43834.338888888888</v>
       </c>
       <c r="K11" s="49"/>
       <c r="L11" s="49"/>
@@ -9734,8 +11047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB39D374-F7E5-4E1B-A824-7220E4B22623}">
   <dimension ref="A2:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>